<commit_message>
wrote allfit tables to csv
</commit_message>
<xml_diff>
--- a/Data/CleanData/YearRandomEffects.xlsx
+++ b/Data/CleanData/YearRandomEffects.xlsx
@@ -1,52 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="forprofit" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="nonprofit" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="government" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="total" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="forprofit" sheetId="1" r:id="rId1"/>
+    <sheet name="nonprofit" sheetId="2" r:id="rId2"/>
+    <sheet name="government" sheetId="3" r:id="rId3"/>
+    <sheet name="total" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intercept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,13 +55,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -128,6 +115,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -153,12 +144,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -184,7 +178,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -360,249 +353,301 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-0.0325994956066216</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>-0.03259949560662156</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B3">
         <v>-0.0117660170303848</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B4">
         <v>-0.0729431256573909</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.000936513324675165</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.0009365133246751645</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.117597837384673</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>0.1175978373846728</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-0.00435602901138277</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>-0.004356029011382772</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.0129458132399659</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.01294581323996592</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B4">
         <v>-0.0473319573286962</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.001994750904905</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.001994750904905001</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B6">
         <v>0.036918166958315</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-0.000981842473638147</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>-0.0009818424736381471</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.010415544289016</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.01041554428901597</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B4">
         <v>-0.0180408423391739</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.00573214290031061</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.005732142900310614</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.00309567806810675</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>0.003095678068106745</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-0.0206739509236922</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>-0.02067395092369222</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>-0.000397720481212945</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>-0.0003977204812129453</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
-        <v>-0.0605640220872632</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>-0.06056402208726316</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.00488675464500182</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.004886754645001824</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.077053716431071</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>0.07705371643107098</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added marijuana to GLM
</commit_message>
<xml_diff>
--- a/Data/CleanData/YearRandomEffects.xlsx
+++ b/Data/CleanData/YearRandomEffects.xlsx
@@ -379,7 +379,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.03259949560662156</v>
+        <v>-0.03466775208093566</v>
       </c>
     </row>
     <row r="3">
@@ -389,7 +389,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.0117660170303848</v>
+        <v>-0.01302760197228154</v>
       </c>
     </row>
     <row r="4">
@@ -399,7 +399,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>-0.0729431256573909</v>
+        <v>-0.07338944145858986</v>
       </c>
     </row>
     <row r="5">
@@ -409,7 +409,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.0009365133246751645</v>
+        <v>0.002206286492960288</v>
       </c>
     </row>
     <row r="6">
@@ -419,7 +419,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.1175978373846728</v>
+        <v>0.1201470517820603</v>
       </c>
     </row>
   </sheetData>
@@ -454,7 +454,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.004356029011382772</v>
+        <v>-0.003085812737391978</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.01294581323996592</v>
+        <v>0.01374037238034471</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>-0.0473319573286962</v>
+        <v>-0.0468626910563708</v>
       </c>
     </row>
     <row r="5">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.001994750904905001</v>
+        <v>0.001042362587145307</v>
       </c>
     </row>
     <row r="6">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.036918166958315</v>
+        <v>0.03537888105551978</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.0009818424736381471</v>
+        <v>-0.001072047097747203</v>
       </c>
     </row>
     <row r="3">
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.01041554428901597</v>
+        <v>0.01050064234067945</v>
       </c>
     </row>
     <row r="4">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>-0.0180408423391739</v>
+        <v>-0.01826618174083947</v>
       </c>
     </row>
     <row r="5">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.005732142900310614</v>
+        <v>0.005880029066311169</v>
       </c>
     </row>
     <row r="6">
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.003095678068106745</v>
+        <v>0.003186633733128033</v>
       </c>
     </row>
   </sheetData>
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.02067395092369222</v>
+        <v>-0.02148302485726171</v>
       </c>
     </row>
     <row r="3">
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.0003977204812129453</v>
+        <v>-0.0008693896351791266</v>
       </c>
     </row>
     <row r="4">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>-0.06056402208726316</v>
+        <v>-0.06070361124259566</v>
       </c>
     </row>
     <row r="5">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.004886754645001824</v>
+        <v>0.005380378932626438</v>
       </c>
     </row>
     <row r="6">
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.07705371643107098</v>
+        <v>0.07798163046410518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>